<commit_message>
dodano zmiane panelu po wykonczeniu wszystkich pytan w quizie.
</commit_message>
<xml_diff>
--- a/Pytania.xlsx
+++ b/Pytania.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="44">
   <si>
     <t>nr</t>
   </si>
@@ -127,6 +127,27 @@
   </si>
   <si>
     <t>wykres_interaktywny_fejsbuk.png</t>
+  </si>
+  <si>
+    <t>Czy gusu przyjmie projek?</t>
+  </si>
+  <si>
+    <t>uep lenie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tak </t>
+  </si>
+  <si>
+    <t>oczywiście estymator krul</t>
+  </si>
+  <si>
+    <t>2.jpg</t>
+  </si>
+  <si>
+    <t>chyba</t>
+  </si>
+  <si>
+    <t>może</t>
   </si>
 </sst>
 </file>
@@ -459,16 +480,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16:H19"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="29.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
     <col min="8" max="8" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1068,6 +1089,162 @@
       </c>
       <c r="H23" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dodano wylaczenie wyboru poziomu trudnosci, gdy wszystkie pytania z bazy zostana zuzyte
</commit_message>
<xml_diff>
--- a/Pytania.xlsx
+++ b/Pytania.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="46">
   <si>
     <t>nr</t>
   </si>
@@ -111,9 +111,6 @@
     <t>WGM</t>
   </si>
   <si>
-    <t>plot/img</t>
-  </si>
-  <si>
     <t>img_src</t>
   </si>
   <si>
@@ -148,6 +145,15 @@
   </si>
   <si>
     <t>może</t>
+  </si>
+  <si>
+    <t>plot_img</t>
+  </si>
+  <si>
+    <t>Ile jest szanys ze to zrobimy?</t>
+  </si>
+  <si>
+    <t>125 i jedna trzecia</t>
   </si>
 </sst>
 </file>
@@ -480,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -513,10 +519,10 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
         <v>31</v>
-      </c>
-      <c r="H1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -542,7 +548,7 @@
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -568,7 +574,7 @@
         <v>8</v>
       </c>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -594,7 +600,7 @@
         <v>8</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -620,7 +626,7 @@
         <v>8</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -646,7 +652,7 @@
         <v>8</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -672,7 +678,7 @@
         <v>8</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -698,7 +704,7 @@
         <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -724,7 +730,7 @@
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -750,7 +756,7 @@
         <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -776,7 +782,7 @@
         <v>8</v>
       </c>
       <c r="H11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -802,7 +808,7 @@
         <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -828,7 +834,7 @@
         <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -854,7 +860,7 @@
         <v>8</v>
       </c>
       <c r="H14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -880,7 +886,7 @@
         <v>8</v>
       </c>
       <c r="H15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -906,7 +912,7 @@
         <v>8</v>
       </c>
       <c r="H16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -932,7 +938,7 @@
         <v>8</v>
       </c>
       <c r="H17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -958,7 +964,7 @@
         <v>8</v>
       </c>
       <c r="H18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -984,7 +990,7 @@
         <v>8</v>
       </c>
       <c r="H19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1010,7 +1016,7 @@
         <v>9</v>
       </c>
       <c r="H20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1036,7 +1042,7 @@
         <v>9</v>
       </c>
       <c r="H21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1062,7 +1068,7 @@
         <v>9</v>
       </c>
       <c r="H22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1088,7 +1094,7 @@
         <v>9</v>
       </c>
       <c r="H23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1102,11 +1108,11 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" t="s">
         <v>37</v>
       </c>
-      <c r="E24" t="s">
-        <v>38</v>
-      </c>
       <c r="F24" t="s">
         <v>8</v>
       </c>
@@ -1114,7 +1120,7 @@
         <v>9</v>
       </c>
       <c r="H24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1128,7 +1134,7 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E25" t="s">
         <v>13</v>
@@ -1140,7 +1146,7 @@
         <v>9</v>
       </c>
       <c r="H25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1154,10 +1160,10 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
@@ -1166,7 +1172,7 @@
         <v>9</v>
       </c>
       <c r="H26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1180,10 +1186,10 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F27" t="s">
         <v>8</v>
@@ -1192,7 +1198,7 @@
         <v>9</v>
       </c>
       <c r="H27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1206,10 +1212,10 @@
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F28" t="s">
         <v>8</v>
@@ -1218,7 +1224,7 @@
         <v>9</v>
       </c>
       <c r="H28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1232,19 +1238,227 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" t="s">
         <v>40</v>
       </c>
-      <c r="F29" t="s">
-        <v>9</v>
-      </c>
-      <c r="G29" t="s">
-        <v>9</v>
-      </c>
-      <c r="H29" t="s">
-        <v>41</v>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>7</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32">
+        <v>5</v>
+      </c>
+      <c r="F32" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33">
+        <v>10</v>
+      </c>
+      <c r="F33" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34">
+        <v>20</v>
+      </c>
+      <c r="F34" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35">
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35">
+        <v>50</v>
+      </c>
+      <c r="F35" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36">
+        <v>7</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36">
+        <v>80</v>
+      </c>
+      <c r="F36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37">
+        <v>7</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
poprawka w poziomie pytan
</commit_message>
<xml_diff>
--- a/Pytania.xlsx
+++ b/Pytania.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="60" windowWidth="11295" windowHeight="5580"/>
@@ -132,8 +132,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,7 +254,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -289,7 +288,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -465,21 +463,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="29.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="47.140625" customWidth="1"/>
+    <col min="5" max="5" width="59.5703125" customWidth="1"/>
     <col min="8" max="8" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -505,7 +503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -531,7 +529,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>1</v>
       </c>
@@ -557,7 +555,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>1</v>
       </c>
@@ -583,7 +581,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>1</v>
       </c>
@@ -609,7 +607,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>3</v>
       </c>
@@ -617,7 +615,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
@@ -635,7 +633,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>3</v>
       </c>
@@ -643,7 +641,7 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
@@ -661,7 +659,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>3</v>
       </c>
@@ -669,7 +667,7 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
@@ -687,7 +685,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>3</v>
       </c>
@@ -695,7 +693,7 @@
         <v>6</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
         <v>18</v>
@@ -713,7 +711,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>4</v>
       </c>
@@ -721,7 +719,7 @@
         <v>6</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
         <v>23</v>
@@ -739,7 +737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>4</v>
       </c>
@@ -747,7 +745,7 @@
         <v>6</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
         <v>23</v>
@@ -765,7 +763,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>4</v>
       </c>
@@ -791,7 +789,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>4</v>
       </c>
@@ -817,7 +815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>5</v>
       </c>
@@ -843,7 +841,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>5</v>
       </c>
@@ -869,7 +867,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>5</v>
       </c>
@@ -895,7 +893,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>5</v>
       </c>
@@ -921,7 +919,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>2</v>
       </c>
@@ -929,7 +927,7 @@
         <v>6</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" t="s">
         <v>35</v>
@@ -947,7 +945,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>2</v>
       </c>
@@ -955,7 +953,7 @@
         <v>6</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
         <v>35</v>
@@ -973,7 +971,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>2</v>
       </c>
@@ -981,7 +979,7 @@
         <v>6</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" t="s">
         <v>35</v>
@@ -993,13 +991,13 @@
         <v>7</v>
       </c>
       <c r="G20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1007,7 +1005,7 @@
         <v>6</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
         <v>35</v>
@@ -1019,13 +1017,13 @@
         <v>7</v>
       </c>
       <c r="G21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1033,7 +1031,7 @@
         <v>6</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
         <v>35</v>
@@ -1045,13 +1043,13 @@
         <v>8</v>
       </c>
       <c r="G22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1059,7 +1057,7 @@
         <v>6</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" t="s">
         <v>35</v>
@@ -1071,7 +1069,7 @@
         <v>7</v>
       </c>
       <c r="G23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H23" t="s">
         <v>36</v>
@@ -1084,12 +1082,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1097,12 +1095,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Dodano trudne pytanie i napisano zdjecie
</commit_message>
<xml_diff>
--- a/Pytania.xlsx
+++ b/Pytania.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="50">
   <si>
     <t>nr</t>
   </si>
@@ -127,6 +127,45 @@
   </si>
   <si>
     <t>img18.jpg</t>
+  </si>
+  <si>
+    <t>gen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which SDG Logo you saw? </t>
+  </si>
+  <si>
+    <t>npov</t>
+  </si>
+  <si>
+    <t>dwaeg</t>
+  </si>
+  <si>
+    <t>Life below water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Life on land </t>
+  </si>
+  <si>
+    <t>pyt_trud.png</t>
+  </si>
+  <si>
+    <t>Affordable and clean energy</t>
+  </si>
+  <si>
+    <t>Zero hunger</t>
+  </si>
+  <si>
+    <t>No poverty</t>
+  </si>
+  <si>
+    <t>Climate action</t>
+  </si>
+  <si>
+    <t>Responsible consumption and production</t>
+  </si>
+  <si>
+    <t>Quality education</t>
   </si>
 </sst>
 </file>
@@ -464,15 +503,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="47.140625" customWidth="1"/>
+    <col min="4" max="4" width="53.28515625" customWidth="1"/>
     <col min="5" max="5" width="59.5703125" customWidth="1"/>
     <col min="8" max="8" width="35.42578125" customWidth="1"/>
   </cols>
@@ -508,7 +547,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -534,7 +573,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -560,7 +599,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -586,7 +625,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -612,7 +651,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -638,7 +677,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -664,7 +703,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -690,7 +729,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -716,7 +755,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -742,7 +781,7 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -768,7 +807,7 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -794,7 +833,7 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -924,7 +963,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -950,7 +989,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -976,7 +1015,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1002,7 +1041,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1028,7 +1067,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1054,7 +1093,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -1073,6 +1112,214 @@
       </c>
       <c r="H23" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dodano polskie komenatrz w :
edkuacja up
global
start serwer
</commit_message>
<xml_diff>
--- a/Pytania.xlsx
+++ b/Pytania.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="50">
   <si>
     <t>nr</t>
   </si>
@@ -39,94 +39,133 @@
     <t>ge</t>
   </si>
   <si>
-    <t>Ile jest 2 + 2?</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
     <t>T</t>
   </si>
   <si>
-    <t xml:space="preserve">Czy lubisz kremowki? </t>
-  </si>
-  <si>
-    <t>NIE</t>
-  </si>
-  <si>
-    <t>NIEEE</t>
-  </si>
-  <si>
-    <t>NIE WIEM</t>
-  </si>
-  <si>
-    <t>CHYBA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAK </t>
-  </si>
-  <si>
-    <t>JESZCZE JAK</t>
-  </si>
-  <si>
-    <t>Jaki dzis dzien?</t>
-  </si>
-  <si>
-    <t>SOBOTA</t>
-  </si>
-  <si>
-    <t>TTr</t>
-  </si>
-  <si>
-    <t>KKK</t>
-  </si>
-  <si>
-    <t>Kangur, pies, kot czy kaczka?</t>
-  </si>
-  <si>
-    <t>kangur</t>
-  </si>
-  <si>
-    <t>pies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kot </t>
-  </si>
-  <si>
-    <t>kaczka</t>
-  </si>
-  <si>
-    <t>Jaki jest najlepszy wydział UEP?</t>
-  </si>
-  <si>
-    <t>WIGE</t>
-  </si>
-  <si>
-    <t>WE</t>
-  </si>
-  <si>
-    <t>WZ</t>
-  </si>
-  <si>
-    <t>WGM</t>
-  </si>
-  <si>
-    <t>plot/img</t>
-  </si>
-  <si>
     <t>img_src</t>
   </si>
   <si>
-    <t>kremufka.jpg</t>
-  </si>
-  <si>
-    <t>1.jpg</t>
-  </si>
-  <si>
     <t>flaga_onztu.png</t>
   </si>
   <si>
-    <t>wykres_interaktywny_fejsbuk.png</t>
+    <t>plot_img</t>
+  </si>
+  <si>
+    <t>plot1.jpg</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Which country has the highest poverty level?</t>
+  </si>
+  <si>
+    <t>Which sentance is true?</t>
+  </si>
+  <si>
+    <t>Growth in Poland is the lowest.</t>
+  </si>
+  <si>
+    <t>Growth in Netherlands is better than in Poland.</t>
+  </si>
+  <si>
+    <t>Germany had no growth in last years.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Growth in Poland is better than in Germany. </t>
+  </si>
+  <si>
+    <t>Which organisation uses this logo?</t>
+  </si>
+  <si>
+    <t>plot3.jpg</t>
+  </si>
+  <si>
+    <t>ONZ</t>
+  </si>
+  <si>
+    <t>UNICEF</t>
+  </si>
+  <si>
+    <t>WHO</t>
+  </si>
+  <si>
+    <t>UE</t>
+  </si>
+  <si>
+    <t>plot2.jpg</t>
+  </si>
+  <si>
+    <t>In which country women held the biggest number of seats?</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Czechia</t>
+  </si>
+  <si>
+    <t>How many SDG there are?</t>
+  </si>
+  <si>
+    <t>img18.jpg</t>
+  </si>
+  <si>
+    <t>gen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which SDG Logo you saw? </t>
+  </si>
+  <si>
+    <t>npov</t>
+  </si>
+  <si>
+    <t>dwaeg</t>
+  </si>
+  <si>
+    <t>Life below water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Life on land </t>
+  </si>
+  <si>
+    <t>pyt_trud.png</t>
+  </si>
+  <si>
+    <t>Affordable and clean energy</t>
+  </si>
+  <si>
+    <t>Zero hunger</t>
+  </si>
+  <si>
+    <t>No poverty</t>
+  </si>
+  <si>
+    <t>Climate action</t>
+  </si>
+  <si>
+    <t>Responsible consumption and production</t>
+  </si>
+  <si>
+    <t>Quality education</t>
   </si>
 </sst>
 </file>
@@ -171,6 +210,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -459,16 +503,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16:H19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="29.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="53.28515625" customWidth="1"/>
+    <col min="5" max="5" width="59.5703125" customWidth="1"/>
     <col min="8" max="8" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -492,10 +536,10 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -503,25 +547,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -529,25 +573,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -555,25 +599,25 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -581,238 +625,238 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
       </c>
       <c r="F5" t="s">
         <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" t="s">
         <v>10</v>
-      </c>
-      <c r="E10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" t="s">
         <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H12" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H13" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -821,24 +865,24 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -847,24 +891,24 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="F15" t="s">
         <v>8</v>
       </c>
       <c r="G15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H15" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -873,24 +917,24 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H16" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -899,42 +943,42 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="F17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H17" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" t="s">
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H18" t="s">
         <v>36</v>
@@ -942,25 +986,25 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" t="s">
-        <v>25</v>
+        <v>35</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H19" t="s">
         <v>36</v>
@@ -968,106 +1012,314 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" t="s">
-        <v>29</v>
+        <v>35</v>
+      </c>
+      <c r="E20">
+        <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" t="s">
-        <v>28</v>
+        <v>35</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G21" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H21" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" t="s">
-        <v>27</v>
+        <v>35</v>
+      </c>
+      <c r="E22">
+        <v>17</v>
       </c>
       <c r="F22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H22" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
         <v>6</v>
       </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" t="s">
         <v>8</v>
       </c>
-      <c r="G23" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" t="s">
-        <v>34</v>
+      <c r="G25" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dodano polska wersje w quizie
</commit_message>
<xml_diff>
--- a/Pytania.xlsx
+++ b/Pytania.xlsx
@@ -60,21 +60,9 @@
     <t>Albania</t>
   </si>
   <si>
-    <t>Portugal</t>
-  </si>
-  <si>
     <t>Ghana</t>
   </si>
   <si>
-    <t>Ethiopia</t>
-  </si>
-  <si>
-    <t>Which country has the highest poverty level?</t>
-  </si>
-  <si>
-    <t>Which sentance is true?</t>
-  </si>
-  <si>
     <t>Growth in Poland is the lowest.</t>
   </si>
   <si>
@@ -87,9 +75,6 @@
     <t xml:space="preserve">Growth in Poland is better than in Germany. </t>
   </si>
   <si>
-    <t>Which organisation uses this logo?</t>
-  </si>
-  <si>
     <t>plot3.jpg</t>
   </si>
   <si>
@@ -108,64 +93,79 @@
     <t>plot2.jpg</t>
   </si>
   <si>
-    <t>In which country women held the biggest number of seats?</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>Denmark</t>
-  </si>
-  <si>
-    <t>Czechia</t>
-  </si>
-  <si>
-    <t>How many SDG there are?</t>
-  </si>
-  <si>
     <t>img18.jpg</t>
   </si>
   <si>
     <t>gen</t>
   </si>
   <si>
-    <t xml:space="preserve">Which SDG Logo you saw? </t>
-  </si>
-  <si>
     <t>npov</t>
   </si>
   <si>
     <t>dwaeg</t>
   </si>
   <si>
-    <t>Life below water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Life on land </t>
-  </si>
-  <si>
     <t>pyt_trud.png</t>
   </si>
   <si>
-    <t>Affordable and clean energy</t>
-  </si>
-  <si>
-    <t>Zero hunger</t>
-  </si>
-  <si>
-    <t>No poverty</t>
-  </si>
-  <si>
-    <t>Climate action</t>
-  </si>
-  <si>
-    <t>Responsible consumption and production</t>
-  </si>
-  <si>
-    <t>Quality education</t>
+    <t>Portugalia</t>
+  </si>
+  <si>
+    <t>Etiopia</t>
+  </si>
+  <si>
+    <t>Który kraj ma najwyzszy poziom wskaźnika biedy?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jakiej organizacji jest to logo? </t>
+  </si>
+  <si>
+    <t>Które zdanie jest prawdziwe?</t>
+  </si>
+  <si>
+    <t>W którym kraju kobiety zajmują najwięcej miejsc w parlamencie?</t>
+  </si>
+  <si>
+    <t>Kanada</t>
+  </si>
+  <si>
+    <t>Francja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Czechy </t>
+  </si>
+  <si>
+    <t>Dania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ile istnieje celów zwrównoważonego rozwoju? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jakiego celu logo zobaczyłeś </t>
+  </si>
+  <si>
+    <t>Zero głodu</t>
+  </si>
+  <si>
+    <t>Życie na lądzie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Koniec z ubstwem </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Działania w dziedzinie klimatu </t>
+  </si>
+  <si>
+    <t>Czysta i dostępna energia</t>
+  </si>
+  <si>
+    <t>Życie pod wodą</t>
+  </si>
+  <si>
+    <t>Dobra jakość edukacji</t>
+  </si>
+  <si>
+    <t>Odpowiedzialna konsumpcja i produkcja</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -547,13 +547,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -573,16 +573,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -599,16 +599,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
@@ -625,16 +625,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
         <v>8</v>
@@ -651,16 +651,16 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
@@ -669,7 +669,7 @@
         <v>7</v>
       </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -677,16 +677,16 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
@@ -695,7 +695,7 @@
         <v>7</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -703,16 +703,16 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
@@ -721,7 +721,7 @@
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -729,25 +729,25 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
         <v>19</v>
-      </c>
-      <c r="F9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -755,16 +755,16 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F10" t="s">
         <v>7</v>
@@ -781,16 +781,16 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
@@ -807,16 +807,16 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F12" t="s">
         <v>7</v>
@@ -833,16 +833,16 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
         <v>23</v>
-      </c>
-      <c r="E13" t="s">
-        <v>28</v>
       </c>
       <c r="F13" t="s">
         <v>7</v>
@@ -865,10 +865,10 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F14" t="s">
         <v>7</v>
@@ -877,7 +877,7 @@
         <v>7</v>
       </c>
       <c r="H14" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -891,10 +891,10 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F15" t="s">
         <v>8</v>
@@ -903,7 +903,7 @@
         <v>7</v>
       </c>
       <c r="H15" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -917,10 +917,10 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s">
         <v>7</v>
@@ -929,7 +929,7 @@
         <v>7</v>
       </c>
       <c r="H16" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -943,10 +943,10 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F17" t="s">
         <v>7</v>
@@ -955,7 +955,7 @@
         <v>7</v>
       </c>
       <c r="H17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -963,13 +963,13 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E18">
         <v>5</v>
@@ -981,7 +981,7 @@
         <v>7</v>
       </c>
       <c r="H18" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -989,13 +989,13 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E19">
         <v>10</v>
@@ -1007,7 +1007,7 @@
         <v>7</v>
       </c>
       <c r="H19" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1015,13 +1015,13 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E20">
         <v>15</v>
@@ -1033,7 +1033,7 @@
         <v>7</v>
       </c>
       <c r="H20" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1041,13 +1041,13 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E21">
         <v>20</v>
@@ -1059,7 +1059,7 @@
         <v>7</v>
       </c>
       <c r="H21" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1067,13 +1067,13 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E22">
         <v>17</v>
@@ -1085,7 +1085,7 @@
         <v>7</v>
       </c>
       <c r="H22" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1093,13 +1093,13 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E23">
         <v>7</v>
@@ -1111,7 +1111,7 @@
         <v>7</v>
       </c>
       <c r="H23" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1119,16 +1119,16 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E24" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F24" t="s">
         <v>7</v>
@@ -1137,7 +1137,7 @@
         <v>7</v>
       </c>
       <c r="H24" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1145,16 +1145,16 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C25">
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E25" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F25" t="s">
         <v>8</v>
@@ -1163,7 +1163,7 @@
         <v>7</v>
       </c>
       <c r="H25" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1171,16 +1171,16 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C26">
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E26" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F26" t="s">
         <v>7</v>
@@ -1189,7 +1189,7 @@
         <v>7</v>
       </c>
       <c r="H26" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1197,16 +1197,16 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C27">
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F27" t="s">
         <v>7</v>
@@ -1215,7 +1215,7 @@
         <v>7</v>
       </c>
       <c r="H27" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1223,16 +1223,16 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C28">
         <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F28" t="s">
         <v>7</v>
@@ -1241,7 +1241,7 @@
         <v>7</v>
       </c>
       <c r="H28" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1249,16 +1249,16 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C29">
         <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F29" t="s">
         <v>7</v>
@@ -1267,7 +1267,7 @@
         <v>7</v>
       </c>
       <c r="H29" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1275,16 +1275,16 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C30">
         <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E30" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F30" t="s">
         <v>7</v>
@@ -1293,7 +1293,7 @@
         <v>7</v>
       </c>
       <c r="H30" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1301,16 +1301,16 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C31">
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F31" t="s">
         <v>7</v>
@@ -1319,7 +1319,7 @@
         <v>7</v>
       </c>
       <c r="H31" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dodano losowanie wybranej przez admina liczby pytan (narzucone w kodzie).
</commit_message>
<xml_diff>
--- a/Pytania.xlsx
+++ b/Pytania.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="83">
   <si>
     <t>nr</t>
   </si>
@@ -166,6 +166,105 @@
   </si>
   <si>
     <t>Odpowiedzialna konsumpcja i produkcja</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Która odp jest dobra?</t>
+  </si>
+  <si>
+    <t>TA</t>
+  </si>
+  <si>
+    <t>Nie TA</t>
+  </si>
+  <si>
+    <t>nie tu</t>
+  </si>
+  <si>
+    <t>nie tam</t>
+  </si>
+  <si>
+    <t>nie nigdzie</t>
+  </si>
+  <si>
+    <t>smutek</t>
+  </si>
+  <si>
+    <t>Jaki był najlepszy utwor Jap poprzedniego sezonu?</t>
+  </si>
+  <si>
+    <t>Silent solitude</t>
+  </si>
+  <si>
+    <t>Innocent note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marionette </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue Bird </t>
+  </si>
+  <si>
+    <t xml:space="preserve">D Techno Life </t>
+  </si>
+  <si>
+    <t>Adamas</t>
+  </si>
+  <si>
+    <t>Sao to bajka?</t>
+  </si>
+  <si>
+    <t>Super</t>
+  </si>
+  <si>
+    <t>Bardzo dobra</t>
+  </si>
+  <si>
+    <t>piec na dziesiec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Powinna się skonczyc </t>
+  </si>
+  <si>
+    <t>Dlaczego ono istnieje</t>
+  </si>
+  <si>
+    <t>Cos się popsulo i nie było go slychac</t>
+  </si>
+  <si>
+    <t>Chyba ok.</t>
+  </si>
+  <si>
+    <t>Trudne pytanka</t>
+  </si>
+  <si>
+    <t>Losowanie to ciezka sprawa</t>
+  </si>
+  <si>
+    <t>Bardzo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bayes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wszystko losowe </t>
+  </si>
+  <si>
+    <t>Nic losowe, wszystko dane</t>
+  </si>
+  <si>
+    <t>Rownania rozniczkowe</t>
+  </si>
+  <si>
+    <t>KHUN TACKER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model dynamiczny arrowa hurtowicza </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kek, herbata się zrobila </t>
   </si>
 </sst>
 </file>
@@ -202,8 +301,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -503,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1320,6 +1420,650 @@
       </c>
       <c r="H31" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35">
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
+        <v>7</v>
+      </c>
+      <c r="B36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" t="s">
+        <v>56</v>
+      </c>
+      <c r="F36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37">
+        <v>7</v>
+      </c>
+      <c r="B37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38">
+        <v>8</v>
+      </c>
+      <c r="B38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" t="s">
+        <v>59</v>
+      </c>
+      <c r="F38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40">
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>58</v>
+      </c>
+      <c r="E40" t="s">
+        <v>61</v>
+      </c>
+      <c r="F40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41" t="s">
+        <v>62</v>
+      </c>
+      <c r="F41" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42">
+        <v>8</v>
+      </c>
+      <c r="B42" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>58</v>
+      </c>
+      <c r="E42" t="s">
+        <v>63</v>
+      </c>
+      <c r="F42" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43">
+        <v>8</v>
+      </c>
+      <c r="B43" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" t="s">
+        <v>64</v>
+      </c>
+      <c r="F43" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44">
+        <v>9</v>
+      </c>
+      <c r="B44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44" t="s">
+        <v>66</v>
+      </c>
+      <c r="F44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45">
+        <v>9</v>
+      </c>
+      <c r="B45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>65</v>
+      </c>
+      <c r="E45" t="s">
+        <v>67</v>
+      </c>
+      <c r="F45" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46">
+        <v>9</v>
+      </c>
+      <c r="B46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46" t="s">
+        <v>65</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F46" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47">
+        <v>9</v>
+      </c>
+      <c r="B47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47" t="s">
+        <v>65</v>
+      </c>
+      <c r="E47" t="s">
+        <v>69</v>
+      </c>
+      <c r="F47" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48">
+        <v>9</v>
+      </c>
+      <c r="B48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48" t="s">
+        <v>70</v>
+      </c>
+      <c r="F48" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49">
+        <v>9</v>
+      </c>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49" t="s">
+        <v>65</v>
+      </c>
+      <c r="E49" t="s">
+        <v>71</v>
+      </c>
+      <c r="F49" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50">
+        <v>9</v>
+      </c>
+      <c r="B50" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50" t="s">
+        <v>72</v>
+      </c>
+      <c r="F50" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51">
+        <v>9</v>
+      </c>
+      <c r="B51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="D51" t="s">
+        <v>65</v>
+      </c>
+      <c r="E51" t="s">
+        <v>73</v>
+      </c>
+      <c r="F51" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52">
+        <v>10</v>
+      </c>
+      <c r="B52" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>74</v>
+      </c>
+      <c r="E52" t="s">
+        <v>75</v>
+      </c>
+      <c r="F52" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53">
+        <v>10</v>
+      </c>
+      <c r="B53" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53" t="s">
+        <v>74</v>
+      </c>
+      <c r="E53" t="s">
+        <v>76</v>
+      </c>
+      <c r="F53" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54">
+        <v>10</v>
+      </c>
+      <c r="B54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="D54" t="s">
+        <v>74</v>
+      </c>
+      <c r="E54" t="s">
+        <v>77</v>
+      </c>
+      <c r="F54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55">
+        <v>10</v>
+      </c>
+      <c r="B55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55" t="s">
+        <v>74</v>
+      </c>
+      <c r="E55" t="s">
+        <v>78</v>
+      </c>
+      <c r="F55" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56">
+        <v>10</v>
+      </c>
+      <c r="B56" t="s">
+        <v>50</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+      <c r="D56" t="s">
+        <v>74</v>
+      </c>
+      <c r="E56" t="s">
+        <v>79</v>
+      </c>
+      <c r="F56" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57">
+        <v>10</v>
+      </c>
+      <c r="B57" t="s">
+        <v>50</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="D57" t="s">
+        <v>74</v>
+      </c>
+      <c r="E57" t="s">
+        <v>80</v>
+      </c>
+      <c r="F57" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58">
+        <v>10</v>
+      </c>
+      <c r="B58" t="s">
+        <v>50</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="D58" t="s">
+        <v>74</v>
+      </c>
+      <c r="E58" t="s">
+        <v>81</v>
+      </c>
+      <c r="F58" t="s">
+        <v>7</v>
+      </c>
+      <c r="G58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59">
+        <v>10</v>
+      </c>
+      <c r="B59" t="s">
+        <v>50</v>
+      </c>
+      <c r="C59">
+        <v>3</v>
+      </c>
+      <c r="D59" t="s">
+        <v>74</v>
+      </c>
+      <c r="E59" t="s">
+        <v>82</v>
+      </c>
+      <c r="F59" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>